<commit_message>
second commit completed full automation script
</commit_message>
<xml_diff>
--- a/Excel/TigerKrionDataSheet.xlsx
+++ b/Excel/TigerKrionDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TWINUser13\eclipse-workspace\check\Krion_6D_Consultation-main\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC56390-626B-4FEB-8C51-B93A5620B720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605FA9C6-BED5-4F9E-8240-C4C163E88665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="3" activeTab="3" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="3" activeTab="8" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="457">
   <si>
     <t>Login Email</t>
   </si>
@@ -1326,9 +1326,6 @@
     <t>Testers</t>
   </si>
   <si>
-    <t>FormTest</t>
-  </si>
-  <si>
     <t>Testdescrption</t>
   </si>
   <si>
@@ -1405,6 +1402,18 @@
   </si>
   <si>
     <t>While creating new project initiallly Parent Review field will have the default template as Select the Parent review after that you can change with any other id</t>
+  </si>
+  <si>
+    <t>Tester61</t>
+  </si>
+  <si>
+    <t>Tester71</t>
+  </si>
+  <si>
+    <t>Tester81</t>
+  </si>
+  <si>
+    <t>For Five Step Approval - Name of Approval will be Answered - its default</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1456,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1493,6 +1502,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1549,7 +1564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1569,6 +1584,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2082,7 +2098,7 @@
         <v>410</v>
       </c>
       <c r="E1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,7 +2120,7 @@
         <v>413</v>
       </c>
       <c r="C3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E3" t="s">
         <v>414</v>
@@ -2115,7 +2131,7 @@
         <v>415</v>
       </c>
       <c r="C4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E4" t="s">
         <v>416</v>
@@ -2126,7 +2142,7 @@
         <v>417</v>
       </c>
       <c r="C5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E5" t="s">
         <v>418</v>
@@ -2137,7 +2153,7 @@
         <v>419</v>
       </c>
       <c r="C6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E6" t="s">
         <v>420</v>
@@ -2148,7 +2164,7 @@
         <v>332</v>
       </c>
       <c r="C7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E7" t="s">
         <v>421</v>
@@ -2159,7 +2175,7 @@
         <v>422</v>
       </c>
       <c r="C8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E8" t="s">
         <v>423</v>
@@ -2369,10 +2385,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B2" t="s">
         <v>449</v>
-      </c>
-      <c r="B2" t="s">
-        <v>450</v>
       </c>
       <c r="C2" t="s">
         <v>339</v>
@@ -2432,7 +2448,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -2527,7 +2543,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
@@ -2679,7 +2695,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
@@ -2970,7 +2986,7 @@
         <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C2" t="s">
         <v>138</v>
@@ -3054,7 +3070,7 @@
         <v>64</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -3271,10 +3287,10 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E2" t="s">
         <v>323</v>
@@ -3355,7 +3371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5927FC2-CAF2-4F62-AF22-9A89FEE1C235}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -3480,10 +3496,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A2A67-EB9E-4636-A126-D12A8CADACD9}">
-  <dimension ref="A1:CJ19"/>
+  <dimension ref="A1:FS23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="AY1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY4" sqref="AY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3918,10 +3934,10 @@
         <v>1</v>
       </c>
       <c r="BF2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH2">
         <v>2</v>
@@ -4094,10 +4110,10 @@
         <v>1</v>
       </c>
       <c r="BF3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH3">
         <v>2</v>
@@ -4282,10 +4298,10 @@
         <v>1</v>
       </c>
       <c r="BF4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH4">
         <v>2</v>
@@ -4462,10 +4478,10 @@
         <v>1</v>
       </c>
       <c r="AY5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BA5">
         <v>1</v>
@@ -4483,10 +4499,10 @@
         <v>1</v>
       </c>
       <c r="BF5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH5">
         <v>2</v>
@@ -4569,205 +4585,160 @@
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>438</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>439</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>441</v>
       </c>
       <c r="F6" t="s">
-        <v>171</v>
+        <v>438</v>
       </c>
       <c r="G6" t="s">
         <v>151</v>
       </c>
       <c r="H6" t="s">
-        <v>233</v>
+        <v>53</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>181</v>
-      </c>
-      <c r="L6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" t="s">
-        <v>182</v>
-      </c>
-      <c r="O6" t="s">
-        <v>183</v>
+        <v>443</v>
       </c>
       <c r="R6" t="s">
-        <v>324</v>
-      </c>
-      <c r="S6" t="s">
-        <v>328</v>
-      </c>
-      <c r="T6" t="s">
-        <v>344</v>
-      </c>
-      <c r="U6" t="s">
-        <v>327</v>
-      </c>
-      <c r="V6" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="AF6" t="s">
-        <v>207</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>208</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>209</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>211</v>
-      </c>
-      <c r="AM6">
-        <v>1</v>
-      </c>
-      <c r="AN6">
-        <v>2</v>
-      </c>
-      <c r="AO6">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="AR6">
         <v>1</v>
       </c>
       <c r="AS6">
+        <v>1</v>
+      </c>
+      <c r="AT6">
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6">
+        <v>1</v>
+      </c>
+      <c r="AX6">
+        <v>1</v>
+      </c>
+      <c r="AY6">
+        <v>1</v>
+      </c>
+      <c r="AZ6">
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>1</v>
+      </c>
+      <c r="BC6">
+        <v>1</v>
+      </c>
+      <c r="BD6">
+        <v>1</v>
+      </c>
+      <c r="BE6">
+        <v>1</v>
+      </c>
+      <c r="BF6">
+        <v>1</v>
+      </c>
+      <c r="BG6">
+        <v>1</v>
+      </c>
+      <c r="BH6">
+        <v>2</v>
+      </c>
+      <c r="BI6">
+        <v>2</v>
+      </c>
+      <c r="BJ6">
+        <v>2</v>
+      </c>
+      <c r="BK6">
+        <v>2</v>
+      </c>
+      <c r="BL6">
+        <v>2</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BQ6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BT6">
+        <v>2</v>
+      </c>
+      <c r="BU6">
+        <v>2</v>
+      </c>
+      <c r="BV6">
+        <v>2</v>
+      </c>
+      <c r="BW6">
+        <v>2</v>
+      </c>
+      <c r="BX6">
+        <v>2</v>
+      </c>
+      <c r="BY6">
+        <v>2</v>
+      </c>
+      <c r="BZ6">
+        <v>2</v>
+      </c>
+      <c r="CA6">
         <v>0</v>
       </c>
-      <c r="AT6">
+      <c r="CB6">
+        <v>1</v>
+      </c>
+      <c r="CC6">
         <v>0</v>
       </c>
-      <c r="AU6">
-        <v>1</v>
-      </c>
-      <c r="AV6">
-        <v>0</v>
-      </c>
-      <c r="AW6">
-        <v>1</v>
-      </c>
-      <c r="AX6">
-        <v>0</v>
-      </c>
-      <c r="AY6">
-        <v>1</v>
-      </c>
-      <c r="AZ6">
-        <v>1</v>
-      </c>
-      <c r="BA6">
-        <v>1</v>
-      </c>
-      <c r="BB6">
-        <v>1</v>
-      </c>
-      <c r="BC6">
-        <v>1</v>
-      </c>
-      <c r="BD6">
-        <v>1</v>
-      </c>
-      <c r="BE6">
-        <v>1</v>
-      </c>
-      <c r="BF6">
-        <v>2</v>
-      </c>
-      <c r="BG6">
-        <v>2</v>
-      </c>
-      <c r="BH6">
-        <v>2</v>
-      </c>
-      <c r="BI6">
-        <v>2</v>
-      </c>
-      <c r="BJ6">
-        <v>2</v>
-      </c>
-      <c r="BK6">
-        <v>2</v>
-      </c>
-      <c r="BL6">
-        <v>2</v>
-      </c>
-      <c r="BM6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BN6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BO6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BP6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BQ6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BR6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BS6" t="s">
-        <v>256</v>
-      </c>
-      <c r="BT6">
-        <v>2</v>
-      </c>
-      <c r="BU6">
-        <v>2</v>
-      </c>
-      <c r="BV6">
-        <v>2</v>
-      </c>
-      <c r="BW6">
-        <v>2</v>
-      </c>
-      <c r="BX6">
-        <v>2</v>
-      </c>
-      <c r="BY6">
-        <v>2</v>
-      </c>
-      <c r="BZ6">
-        <v>2</v>
-      </c>
-      <c r="CA6">
-        <v>1</v>
-      </c>
-      <c r="CB6">
-        <v>0</v>
-      </c>
-      <c r="CC6">
-        <v>1</v>
-      </c>
       <c r="CD6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE6">
         <v>1</v>
@@ -4781,22 +4752,22 @@
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>438</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>440</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>442</v>
       </c>
       <c r="F7" t="s">
-        <v>178</v>
+        <v>438</v>
       </c>
       <c r="G7" t="s">
         <v>151</v>
@@ -4808,75 +4779,17 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K7" t="s">
-        <v>186</v>
-      </c>
-      <c r="L7" t="s">
-        <v>187</v>
-      </c>
-      <c r="M7" t="s">
-        <v>188</v>
-      </c>
-      <c r="N7" t="s">
-        <v>189</v>
-      </c>
-      <c r="O7" t="s">
-        <v>190</v>
-      </c>
-      <c r="P7" t="s">
-        <v>191</v>
+        <v>444</v>
       </c>
       <c r="R7" t="s">
         <v>326</v>
       </c>
-      <c r="S7" t="s">
-        <v>157</v>
-      </c>
-      <c r="T7" t="s">
-        <v>324</v>
-      </c>
-      <c r="U7" t="s">
-        <v>328</v>
-      </c>
-      <c r="V7" t="s">
-        <v>345</v>
-      </c>
-      <c r="W7" t="s">
-        <v>329</v>
-      </c>
-      <c r="AC7" s="5"/>
       <c r="AF7" t="s">
         <v>62</v>
       </c>
-      <c r="AG7" t="s">
-        <v>234</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>235</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>236</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>237</v>
-      </c>
-      <c r="AM7">
-        <v>1</v>
-      </c>
-      <c r="AN7">
-        <v>1</v>
-      </c>
-      <c r="AO7">
-        <v>2</v>
-      </c>
-      <c r="AP7">
-        <v>2</v>
-      </c>
       <c r="AR7">
         <v>1</v>
       </c>
@@ -4890,103 +4803,103 @@
         <v>1</v>
       </c>
       <c r="AV7">
+        <v>1</v>
+      </c>
+      <c r="AW7">
+        <v>1</v>
+      </c>
+      <c r="AX7">
+        <v>1</v>
+      </c>
+      <c r="AY7">
+        <v>1</v>
+      </c>
+      <c r="AZ7">
+        <v>1</v>
+      </c>
+      <c r="BA7">
+        <v>1</v>
+      </c>
+      <c r="BB7">
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <v>1</v>
+      </c>
+      <c r="BD7">
+        <v>1</v>
+      </c>
+      <c r="BE7">
+        <v>1</v>
+      </c>
+      <c r="BF7">
+        <v>1</v>
+      </c>
+      <c r="BG7">
+        <v>1</v>
+      </c>
+      <c r="BH7">
+        <v>2</v>
+      </c>
+      <c r="BI7">
+        <v>2</v>
+      </c>
+      <c r="BJ7">
+        <v>2</v>
+      </c>
+      <c r="BK7">
+        <v>2</v>
+      </c>
+      <c r="BL7">
+        <v>2</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BO7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BQ7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>256</v>
+      </c>
+      <c r="BT7">
+        <v>2</v>
+      </c>
+      <c r="BU7">
+        <v>2</v>
+      </c>
+      <c r="BV7">
+        <v>2</v>
+      </c>
+      <c r="BW7">
+        <v>2</v>
+      </c>
+      <c r="BX7">
+        <v>2</v>
+      </c>
+      <c r="BY7">
+        <v>2</v>
+      </c>
+      <c r="BZ7">
+        <v>2</v>
+      </c>
+      <c r="CA7">
         <v>0</v>
       </c>
-      <c r="AW7">
-        <v>0</v>
-      </c>
-      <c r="AX7">
-        <v>1</v>
-      </c>
-      <c r="AY7">
-        <v>1</v>
-      </c>
-      <c r="AZ7">
-        <v>1</v>
-      </c>
-      <c r="BA7">
-        <v>1</v>
-      </c>
-      <c r="BB7">
-        <v>1</v>
-      </c>
-      <c r="BC7">
-        <v>1</v>
-      </c>
-      <c r="BD7">
-        <v>1</v>
-      </c>
-      <c r="BE7">
-        <v>1</v>
-      </c>
-      <c r="BF7">
-        <v>2</v>
-      </c>
-      <c r="BG7">
-        <v>2</v>
-      </c>
-      <c r="BH7">
-        <v>2</v>
-      </c>
-      <c r="BI7">
-        <v>2</v>
-      </c>
-      <c r="BJ7">
-        <v>2</v>
-      </c>
-      <c r="BK7">
-        <v>2</v>
-      </c>
-      <c r="BL7">
-        <v>2</v>
-      </c>
-      <c r="BM7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BN7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BO7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BP7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BQ7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BR7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BS7" t="s">
-        <v>256</v>
-      </c>
-      <c r="BT7">
-        <v>2</v>
-      </c>
-      <c r="BU7">
-        <v>2</v>
-      </c>
-      <c r="BV7">
-        <v>2</v>
-      </c>
-      <c r="BW7">
-        <v>2</v>
-      </c>
-      <c r="BX7">
-        <v>2</v>
-      </c>
-      <c r="BY7">
-        <v>2</v>
-      </c>
-      <c r="BZ7">
-        <v>2</v>
-      </c>
-      <c r="CA7">
-        <v>1</v>
-      </c>
       <c r="CB7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC7">
         <v>0</v>
@@ -4995,10 +4908,10 @@
         <v>1</v>
       </c>
       <c r="CE7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG7">
         <v>1</v>
@@ -5006,117 +4919,46 @@
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>193</v>
+        <v>441</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="G8" t="s">
         <v>151</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>233</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>194</v>
-      </c>
-      <c r="L8" t="s">
-        <v>195</v>
-      </c>
-      <c r="M8" t="s">
-        <v>196</v>
-      </c>
-      <c r="N8" t="s">
-        <v>197</v>
-      </c>
-      <c r="O8" t="s">
-        <v>198</v>
-      </c>
-      <c r="P8" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="R8" t="s">
-        <v>344</v>
-      </c>
-      <c r="S8" t="s">
-        <v>157</v>
-      </c>
-      <c r="T8" t="s">
-        <v>345</v>
-      </c>
-      <c r="U8" t="s">
         <v>326</v>
       </c>
-      <c r="V8" t="s">
-        <v>346</v>
-      </c>
-      <c r="W8" t="s">
-        <v>328</v>
-      </c>
-      <c r="X8" t="s">
-        <v>324</v>
-      </c>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
       <c r="AF8" t="s">
-        <v>348</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>349</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>350</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>351</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>352</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>353</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>354</v>
-      </c>
-      <c r="AM8">
-        <v>2</v>
-      </c>
-      <c r="AN8">
-        <v>1</v>
-      </c>
-      <c r="AO8">
-        <v>1</v>
-      </c>
-      <c r="AP8">
-        <v>2</v>
-      </c>
-      <c r="AQ8">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="AR8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS8">
         <v>1</v>
@@ -5125,10 +4967,10 @@
         <v>1</v>
       </c>
       <c r="AU8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW8">
         <v>1</v>
@@ -5158,25 +5000,25 @@
         <v>1</v>
       </c>
       <c r="BF8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BI8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BJ8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BK8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BL8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BM8" t="s">
         <v>256</v>
@@ -5200,31 +5042,31 @@
         <v>256</v>
       </c>
       <c r="BT8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BU8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BV8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BW8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BX8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BY8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BZ8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CA8">
         <v>0</v>
       </c>
       <c r="CB8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC8">
         <v>0</v>
@@ -5233,18 +5075,18 @@
         <v>1</v>
       </c>
       <c r="CE8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF8">
         <v>1</v>
       </c>
       <c r="CG8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>439</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
@@ -5253,13 +5095,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>440</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
         <v>442</v>
       </c>
       <c r="F9" t="s">
-        <v>439</v>
+        <v>178</v>
       </c>
       <c r="G9" t="s">
         <v>151</v>
@@ -5274,7 +5116,7 @@
         <v>56</v>
       </c>
       <c r="K9" t="s">
-        <v>444</v>
+        <v>186</v>
       </c>
       <c r="R9" t="s">
         <v>326</v>
@@ -5325,25 +5167,25 @@
         <v>1</v>
       </c>
       <c r="BF9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BI9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BJ9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BK9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BL9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BM9" t="s">
         <v>256</v>
@@ -5367,25 +5209,25 @@
         <v>256</v>
       </c>
       <c r="BT9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BU9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BV9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BW9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BX9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BY9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BZ9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CA9">
         <v>0</v>
@@ -5397,7 +5239,7 @@
         <v>0</v>
       </c>
       <c r="CD9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE9">
         <v>1</v>
@@ -5411,7 +5253,7 @@
     </row>
     <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>439</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>56</v>
@@ -5420,13 +5262,13 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>441</v>
+        <v>192</v>
       </c>
       <c r="E10" t="s">
-        <v>443</v>
+        <v>173</v>
       </c>
       <c r="F10" t="s">
-        <v>439</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
         <v>151</v>
@@ -5441,7 +5283,7 @@
         <v>56</v>
       </c>
       <c r="K10" t="s">
-        <v>445</v>
+        <v>194</v>
       </c>
       <c r="R10" t="s">
         <v>326</v>
@@ -5492,25 +5334,25 @@
         <v>1</v>
       </c>
       <c r="BF10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BI10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BJ10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BK10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BL10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BM10" t="s">
         <v>256</v>
@@ -5534,28 +5376,28 @@
         <v>256</v>
       </c>
       <c r="BT10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BU10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BV10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BW10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BX10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BY10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BZ10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CA10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB10">
         <v>1</v>
@@ -5564,7 +5406,7 @@
         <v>0</v>
       </c>
       <c r="CD10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE10">
         <v>1</v>
@@ -5576,231 +5418,903 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="I16" s="9" t="s">
+    <row r="20" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="I20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AR16" s="9" t="s">
+      <c r="AR20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AS16" s="9" t="s">
+      <c r="AS20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AT16" s="9" t="s">
+      <c r="AT20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AU16" s="9" t="s">
+      <c r="AU20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AV16" s="9" t="s">
+      <c r="AV20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AW16" s="9" t="s">
+      <c r="AW20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="AX16" s="9" t="s">
+      <c r="AX20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BM16" s="9" t="s">
+      <c r="BM20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BN16" s="9" t="s">
+      <c r="BN20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BO16" s="9" t="s">
+      <c r="BO20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BP16" s="9" t="s">
+      <c r="BP20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BQ16" s="9" t="s">
+      <c r="BQ20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BR16" s="9" t="s">
+      <c r="BR20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="BS16" s="9" t="s">
+      <c r="BS20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CA16" s="9" t="s">
+      <c r="CA20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CB16" s="9" t="s">
+      <c r="CB20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CC16" s="9" t="s">
+      <c r="CC20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CD16" s="9" t="s">
+      <c r="CD20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CE16" s="9" t="s">
+      <c r="CE20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CF16" s="9" t="s">
+      <c r="CF20" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="CG16" s="9" t="s">
+      <c r="CG20" s="9" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="9:85" x14ac:dyDescent="0.25">
-      <c r="I17" s="11" t="s">
+    <row r="21" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="I21" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="AR17" s="11" t="s">
+      <c r="AR21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="AS17" s="11" t="s">
+      <c r="AS21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="AT17" s="11" t="s">
+      <c r="AT21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="AU17" s="11" t="s">
+      <c r="AU21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="AV17" s="11" t="s">
+      <c r="AV21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="AW17" s="11" t="s">
+      <c r="AW21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="AX17" s="11" t="s">
+      <c r="AX21" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="BM17" s="11" t="s">
+      <c r="BM21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="BN17" s="11" t="s">
+      <c r="BN21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="BO17" s="11" t="s">
+      <c r="BO21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="BP17" s="11" t="s">
+      <c r="BP21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="BQ17" s="11" t="s">
+      <c r="BQ21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="BR17" s="11" t="s">
+      <c r="BR21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="BS17" s="11" t="s">
+      <c r="BS21" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="CA17" s="11" t="s">
+      <c r="CA21" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="CB17" s="11" t="s">
+      <c r="CB21" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="CC17" s="11" t="s">
+      <c r="CC21" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="CD17" s="11" t="s">
+      <c r="CD21" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="CE17" s="11" t="s">
+      <c r="CE21" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="CF17" s="11" t="s">
+      <c r="CF21" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="CG17" s="11" t="s">
+      <c r="CG21" s="11" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="18" spans="9:85" x14ac:dyDescent="0.25">
-      <c r="I18" s="11" t="s">
+      <c r="CM21" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="CN21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="CO21" s="19">
+        <v>5</v>
+      </c>
+      <c r="CP21" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="CQ21" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="CR21" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="CS21" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="CT21" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="CU21">
+        <v>1</v>
+      </c>
+      <c r="CV21" t="s">
+        <v>58</v>
+      </c>
+      <c r="CW21" t="s">
+        <v>181</v>
+      </c>
+      <c r="CX21" t="s">
+        <v>138</v>
+      </c>
+      <c r="CY21" t="s">
+        <v>51</v>
+      </c>
+      <c r="CZ21" t="s">
+        <v>182</v>
+      </c>
+      <c r="DA21" t="s">
+        <v>183</v>
+      </c>
+      <c r="DD21" t="s">
+        <v>324</v>
+      </c>
+      <c r="DE21" t="s">
+        <v>328</v>
+      </c>
+      <c r="DF21" t="s">
+        <v>344</v>
+      </c>
+      <c r="DG21" t="s">
+        <v>327</v>
+      </c>
+      <c r="DH21" t="s">
+        <v>345</v>
+      </c>
+      <c r="DR21" t="s">
+        <v>207</v>
+      </c>
+      <c r="DS21" t="s">
+        <v>208</v>
+      </c>
+      <c r="DT21" t="s">
+        <v>209</v>
+      </c>
+      <c r="DU21" t="s">
+        <v>210</v>
+      </c>
+      <c r="DV21" t="s">
+        <v>211</v>
+      </c>
+      <c r="DY21">
+        <v>1</v>
+      </c>
+      <c r="DZ21">
+        <v>2</v>
+      </c>
+      <c r="EA21">
+        <v>2</v>
+      </c>
+      <c r="ED21">
+        <v>1</v>
+      </c>
+      <c r="EE21">
+        <v>0</v>
+      </c>
+      <c r="EF21">
+        <v>0</v>
+      </c>
+      <c r="EG21">
+        <v>1</v>
+      </c>
+      <c r="EH21">
+        <v>0</v>
+      </c>
+      <c r="EI21">
+        <v>1</v>
+      </c>
+      <c r="EJ21">
+        <v>0</v>
+      </c>
+      <c r="EK21">
+        <v>1</v>
+      </c>
+      <c r="EL21">
+        <v>1</v>
+      </c>
+      <c r="EM21">
+        <v>1</v>
+      </c>
+      <c r="EN21">
+        <v>1</v>
+      </c>
+      <c r="EO21">
+        <v>1</v>
+      </c>
+      <c r="EP21">
+        <v>1</v>
+      </c>
+      <c r="EQ21">
+        <v>1</v>
+      </c>
+      <c r="ER21">
+        <v>2</v>
+      </c>
+      <c r="ES21">
+        <v>2</v>
+      </c>
+      <c r="ET21">
+        <v>2</v>
+      </c>
+      <c r="EU21">
+        <v>2</v>
+      </c>
+      <c r="EV21">
+        <v>2</v>
+      </c>
+      <c r="EW21">
+        <v>2</v>
+      </c>
+      <c r="EX21">
+        <v>2</v>
+      </c>
+      <c r="EY21" t="s">
+        <v>256</v>
+      </c>
+      <c r="EZ21" t="s">
+        <v>256</v>
+      </c>
+      <c r="FA21" t="s">
+        <v>256</v>
+      </c>
+      <c r="FB21" t="s">
+        <v>256</v>
+      </c>
+      <c r="FC21" t="s">
+        <v>256</v>
+      </c>
+      <c r="FD21" t="s">
+        <v>256</v>
+      </c>
+      <c r="FE21" t="s">
+        <v>256</v>
+      </c>
+      <c r="FF21">
+        <v>2</v>
+      </c>
+      <c r="FG21">
+        <v>2</v>
+      </c>
+      <c r="FH21">
+        <v>2</v>
+      </c>
+      <c r="FI21">
+        <v>2</v>
+      </c>
+      <c r="FJ21">
+        <v>2</v>
+      </c>
+      <c r="FK21">
+        <v>2</v>
+      </c>
+      <c r="FL21">
+        <v>2</v>
+      </c>
+      <c r="FM21">
+        <v>1</v>
+      </c>
+      <c r="FN21">
+        <v>0</v>
+      </c>
+      <c r="FO21">
+        <v>1</v>
+      </c>
+      <c r="FP21">
+        <v>0</v>
+      </c>
+      <c r="FQ21">
+        <v>1</v>
+      </c>
+      <c r="FR21">
+        <v>1</v>
+      </c>
+      <c r="FS21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="I22" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="AR18" s="11" t="s">
+      <c r="AR22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="AS18" s="11" t="s">
+      <c r="AS22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="AT18" s="11" t="s">
+      <c r="AT22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="AU18" s="11" t="s">
+      <c r="AU22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="AV18" s="11" t="s">
+      <c r="AV22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="AW18" s="11" t="s">
+      <c r="AW22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="AX18" s="11" t="s">
+      <c r="AX22" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="BM18" s="11" t="s">
+      <c r="BM22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="BN18" s="11" t="s">
+      <c r="BN22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="BO18" s="11" t="s">
+      <c r="BO22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="BP18" s="11" t="s">
+      <c r="BP22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="BQ18" s="11" t="s">
+      <c r="BQ22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="BR18" s="11" t="s">
+      <c r="BR22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="BS18" s="11" t="s">
+      <c r="BS22" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="CA18" s="11" t="s">
+      <c r="CA22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="CB18" s="11" t="s">
+      <c r="CB22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="CC18" s="11" t="s">
+      <c r="CC22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="CD18" s="11" t="s">
+      <c r="CD22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="CE18" s="11" t="s">
+      <c r="CE22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="CF18" s="11" t="s">
+      <c r="CF22" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="CG18" s="11" t="s">
+      <c r="CG22" s="11" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="19" spans="9:85" x14ac:dyDescent="0.25">
-      <c r="BM19" s="11" t="s">
+      <c r="CM22" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="CN22" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="CO22" s="19">
+        <v>6</v>
+      </c>
+      <c r="CP22" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="CQ22" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="CR22" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="CS22" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="CT22" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CU22">
+        <v>1</v>
+      </c>
+      <c r="CV22" t="s">
+        <v>59</v>
+      </c>
+      <c r="CW22" t="s">
+        <v>186</v>
+      </c>
+      <c r="CX22" t="s">
+        <v>187</v>
+      </c>
+      <c r="CY22" t="s">
+        <v>188</v>
+      </c>
+      <c r="CZ22" t="s">
+        <v>189</v>
+      </c>
+      <c r="DA22" t="s">
+        <v>190</v>
+      </c>
+      <c r="DB22" t="s">
+        <v>191</v>
+      </c>
+      <c r="DD22" t="s">
+        <v>326</v>
+      </c>
+      <c r="DE22" t="s">
+        <v>157</v>
+      </c>
+      <c r="DF22" t="s">
+        <v>324</v>
+      </c>
+      <c r="DG22" t="s">
+        <v>328</v>
+      </c>
+      <c r="DH22" t="s">
+        <v>345</v>
+      </c>
+      <c r="DI22" t="s">
+        <v>329</v>
+      </c>
+      <c r="DO22" s="5"/>
+      <c r="DR22" t="s">
+        <v>62</v>
+      </c>
+      <c r="DS22" t="s">
+        <v>234</v>
+      </c>
+      <c r="DT22" t="s">
+        <v>235</v>
+      </c>
+      <c r="DU22" t="s">
+        <v>236</v>
+      </c>
+      <c r="DV22" t="s">
+        <v>62</v>
+      </c>
+      <c r="DW22" t="s">
+        <v>237</v>
+      </c>
+      <c r="DY22">
+        <v>1</v>
+      </c>
+      <c r="DZ22">
+        <v>1</v>
+      </c>
+      <c r="EA22">
+        <v>2</v>
+      </c>
+      <c r="EB22">
+        <v>2</v>
+      </c>
+      <c r="ED22">
+        <v>1</v>
+      </c>
+      <c r="EE22">
+        <v>1</v>
+      </c>
+      <c r="EF22">
+        <v>1</v>
+      </c>
+      <c r="EG22">
+        <v>1</v>
+      </c>
+      <c r="EH22">
+        <v>0</v>
+      </c>
+      <c r="EI22">
+        <v>0</v>
+      </c>
+      <c r="EJ22">
+        <v>1</v>
+      </c>
+      <c r="EK22">
+        <v>1</v>
+      </c>
+      <c r="EL22">
+        <v>1</v>
+      </c>
+      <c r="EM22">
+        <v>1</v>
+      </c>
+      <c r="EN22">
+        <v>1</v>
+      </c>
+      <c r="EO22">
+        <v>1</v>
+      </c>
+      <c r="EP22">
+        <v>1</v>
+      </c>
+      <c r="EQ22">
+        <v>1</v>
+      </c>
+      <c r="ER22">
+        <v>2</v>
+      </c>
+      <c r="ES22">
+        <v>2</v>
+      </c>
+      <c r="ET22">
+        <v>2</v>
+      </c>
+      <c r="EU22">
+        <v>2</v>
+      </c>
+      <c r="EV22">
+        <v>2</v>
+      </c>
+      <c r="EW22">
+        <v>2</v>
+      </c>
+      <c r="EX22">
+        <v>2</v>
+      </c>
+      <c r="EY22" t="s">
+        <v>256</v>
+      </c>
+      <c r="EZ22" t="s">
+        <v>256</v>
+      </c>
+      <c r="FA22" t="s">
+        <v>256</v>
+      </c>
+      <c r="FB22" t="s">
+        <v>256</v>
+      </c>
+      <c r="FC22" t="s">
+        <v>256</v>
+      </c>
+      <c r="FD22" t="s">
+        <v>256</v>
+      </c>
+      <c r="FE22" t="s">
+        <v>256</v>
+      </c>
+      <c r="FF22">
+        <v>2</v>
+      </c>
+      <c r="FG22">
+        <v>2</v>
+      </c>
+      <c r="FH22">
+        <v>2</v>
+      </c>
+      <c r="FI22">
+        <v>2</v>
+      </c>
+      <c r="FJ22">
+        <v>2</v>
+      </c>
+      <c r="FK22">
+        <v>2</v>
+      </c>
+      <c r="FL22">
+        <v>2</v>
+      </c>
+      <c r="FM22">
+        <v>1</v>
+      </c>
+      <c r="FN22">
+        <v>0</v>
+      </c>
+      <c r="FO22">
+        <v>0</v>
+      </c>
+      <c r="FP22">
+        <v>1</v>
+      </c>
+      <c r="FQ22">
+        <v>0</v>
+      </c>
+      <c r="FR22">
+        <v>0</v>
+      </c>
+      <c r="FS22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="I23" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="BM23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="BN19" s="11" t="s">
+      <c r="BN23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="BO19" s="11" t="s">
+      <c r="BO23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="BP19" s="11" t="s">
+      <c r="BP23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="BQ19" s="11" t="s">
+      <c r="BQ23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="BR19" s="11" t="s">
+      <c r="BR23" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="BS19" s="11" t="s">
+      <c r="BS23" s="11" t="s">
         <v>319</v>
+      </c>
+      <c r="CM23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="CN23" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="CO23" s="19">
+        <v>7</v>
+      </c>
+      <c r="CP23" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="CQ23" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="CR23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="CS23" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="CT23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CU23">
+        <v>0</v>
+      </c>
+      <c r="CV23" t="s">
+        <v>60</v>
+      </c>
+      <c r="CW23" t="s">
+        <v>194</v>
+      </c>
+      <c r="CX23" t="s">
+        <v>195</v>
+      </c>
+      <c r="CY23" t="s">
+        <v>196</v>
+      </c>
+      <c r="CZ23" t="s">
+        <v>197</v>
+      </c>
+      <c r="DA23" t="s">
+        <v>198</v>
+      </c>
+      <c r="DB23" t="s">
+        <v>199</v>
+      </c>
+      <c r="DC23" t="s">
+        <v>200</v>
+      </c>
+      <c r="DD23" t="s">
+        <v>344</v>
+      </c>
+      <c r="DE23" t="s">
+        <v>157</v>
+      </c>
+      <c r="DF23" t="s">
+        <v>345</v>
+      </c>
+      <c r="DG23" t="s">
+        <v>326</v>
+      </c>
+      <c r="DH23" t="s">
+        <v>346</v>
+      </c>
+      <c r="DI23" t="s">
+        <v>328</v>
+      </c>
+      <c r="DJ23" t="s">
+        <v>324</v>
+      </c>
+      <c r="DO23" s="5"/>
+      <c r="DP23" s="5"/>
+      <c r="DR23" t="s">
+        <v>348</v>
+      </c>
+      <c r="DS23" t="s">
+        <v>349</v>
+      </c>
+      <c r="DT23" t="s">
+        <v>350</v>
+      </c>
+      <c r="DU23" t="s">
+        <v>351</v>
+      </c>
+      <c r="DV23" t="s">
+        <v>352</v>
+      </c>
+      <c r="DW23" t="s">
+        <v>353</v>
+      </c>
+      <c r="DX23" t="s">
+        <v>354</v>
+      </c>
+      <c r="DY23">
+        <v>2</v>
+      </c>
+      <c r="DZ23">
+        <v>1</v>
+      </c>
+      <c r="EA23">
+        <v>1</v>
+      </c>
+      <c r="EB23">
+        <v>2</v>
+      </c>
+      <c r="EC23">
+        <v>2</v>
+      </c>
+      <c r="ED23">
+        <v>2</v>
+      </c>
+      <c r="EE23">
+        <v>1</v>
+      </c>
+      <c r="EF23">
+        <v>1</v>
+      </c>
+      <c r="EG23">
+        <v>0</v>
+      </c>
+      <c r="EH23">
+        <v>0</v>
+      </c>
+      <c r="EI23">
+        <v>1</v>
+      </c>
+      <c r="EJ23">
+        <v>1</v>
+      </c>
+      <c r="EK23">
+        <v>1</v>
+      </c>
+      <c r="EL23">
+        <v>1</v>
+      </c>
+      <c r="EM23">
+        <v>1</v>
+      </c>
+      <c r="EN23">
+        <v>1</v>
+      </c>
+      <c r="EO23">
+        <v>1</v>
+      </c>
+      <c r="EP23">
+        <v>1</v>
+      </c>
+      <c r="EQ23">
+        <v>1</v>
+      </c>
+      <c r="ER23">
+        <v>2</v>
+      </c>
+      <c r="ES23">
+        <v>2</v>
+      </c>
+      <c r="ET23">
+        <v>2</v>
+      </c>
+      <c r="EU23">
+        <v>2</v>
+      </c>
+      <c r="EV23">
+        <v>2</v>
+      </c>
+      <c r="EW23">
+        <v>2</v>
+      </c>
+      <c r="EX23">
+        <v>2</v>
+      </c>
+      <c r="EY23" t="s">
+        <v>256</v>
+      </c>
+      <c r="EZ23" t="s">
+        <v>256</v>
+      </c>
+      <c r="FA23" t="s">
+        <v>256</v>
+      </c>
+      <c r="FB23" t="s">
+        <v>256</v>
+      </c>
+      <c r="FC23" t="s">
+        <v>256</v>
+      </c>
+      <c r="FD23" t="s">
+        <v>256</v>
+      </c>
+      <c r="FE23" t="s">
+        <v>256</v>
+      </c>
+      <c r="FF23">
+        <v>2</v>
+      </c>
+      <c r="FG23">
+        <v>2</v>
+      </c>
+      <c r="FH23">
+        <v>2</v>
+      </c>
+      <c r="FI23">
+        <v>2</v>
+      </c>
+      <c r="FJ23">
+        <v>2</v>
+      </c>
+      <c r="FK23">
+        <v>2</v>
+      </c>
+      <c r="FL23">
+        <v>2</v>
+      </c>
+      <c r="FM23">
+        <v>0</v>
+      </c>
+      <c r="FN23">
+        <v>1</v>
+      </c>
+      <c r="FO23">
+        <v>0</v>
+      </c>
+      <c r="FP23">
+        <v>1</v>
+      </c>
+      <c r="FQ23">
+        <v>0</v>
+      </c>
+      <c r="FR23">
+        <v>1</v>
+      </c>
+      <c r="FS23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5899,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D2" t="s">
         <v>364</v>
@@ -6070,7 +6584,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D2" t="s">
         <v>383</v>
@@ -6088,7 +6602,7 @@
         <v>386</v>
       </c>
       <c r="I2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J2">
         <v>30</v>
@@ -6203,7 +6717,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D2" t="s">
         <v>389</v>
@@ -6212,7 +6726,7 @@
         <v>426</v>
       </c>
       <c r="F2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G2" t="s">
         <v>425</v>
@@ -6230,8 +6744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF25439C-7A3F-4F80-9A72-7D557AD94E32}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6354,10 +6868,10 @@
         <v>365</v>
       </c>
       <c r="J2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" t="s">
         <v>427</v>
-      </c>
-      <c r="K2" t="s">
-        <v>428</v>
       </c>
       <c r="M2" t="s">
         <v>404</v>

</xml_diff>

<commit_message>
Document module issue resloved
</commit_message>
<xml_diff>
--- a/Excel/TigerKrionDataSheet.xlsx
+++ b/Excel/TigerKrionDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TWINUser13\eclipse-workspace\check\Krion_6D_Consultation-main\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605FA9C6-BED5-4F9E-8240-C4C163E88665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6445EFE2-7FA0-49EF-87CD-2BEFB9D7A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="3" activeTab="8" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="454">
   <si>
     <t>Login Email</t>
   </si>
@@ -978,27 +978,15 @@
     <t>Estimated Total, Quoted Total, Actual Total are calculated based on the before two field valid by the code</t>
   </si>
   <si>
-    <t>1 - Ticks the Editable CheckBox</t>
-  </si>
-  <si>
     <t>0 - UnTicks the Editable CheckBox</t>
   </si>
   <si>
-    <t>1 - Ticks the EmailTrigger CheckBox</t>
-  </si>
-  <si>
     <t>0 - UnTicks the Email Trigger CheckBox</t>
   </si>
   <si>
-    <t>1 - Ticks Minimum Number Of Members Required Radio Button</t>
-  </si>
-  <si>
     <t>0 - Ticks Every member must review</t>
   </si>
   <si>
-    <t>There are Two Options</t>
-  </si>
-  <si>
     <t>1. Calendar Day</t>
   </si>
   <si>
@@ -1020,9 +1008,6 @@
     <t>Kesavan 1234</t>
   </si>
   <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
     <t>Ayyamperumal T</t>
   </si>
   <si>
@@ -1038,9 +1023,6 @@
     <t>Full Control</t>
   </si>
   <si>
-    <t>Consultant</t>
-  </si>
-  <si>
     <t>Electrical</t>
   </si>
   <si>
@@ -1065,15 +1047,6 @@
     <t>Gokipal</t>
   </si>
   <si>
-    <t>Kriuba Krion</t>
-  </si>
-  <si>
-    <t>WATCHER</t>
-  </si>
-  <si>
-    <t>Project viewer</t>
-  </si>
-  <si>
     <t>TestConsultant</t>
   </si>
   <si>
@@ -1281,42 +1254,21 @@
     <t>Imag</t>
   </si>
   <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\dwsample-jpeg-1280</t>
-  </si>
-  <si>
     <t>Floor</t>
   </si>
   <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\FloorPlan.dwg</t>
-  </si>
-  <si>
     <t>MHV</t>
   </si>
   <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\MHV 2024.rvt</t>
-  </si>
-  <si>
     <t>Interior</t>
   </si>
   <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\56750_A_2024_INTERIOR ELEVATIONS.pdf</t>
-  </si>
-  <si>
     <t>industry</t>
   </si>
   <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\industry</t>
-  </si>
-  <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\Snowdon Towers Sample Electrical.rvt</t>
-  </si>
-  <si>
     <t>Only roof</t>
   </si>
   <si>
-    <t>C:\Users\TWINUser-08\Desktop\Project Documents\Snowdon Towers Sample Structural_Metric pm1-3D View - Structure Only Roof.dwg</t>
-  </si>
-  <si>
     <t>Site Engineer</t>
   </si>
   <si>
@@ -1329,9 +1281,6 @@
     <t>Testdescrption</t>
   </si>
   <si>
-    <t>Documentpath1</t>
-  </si>
-  <si>
     <t>C:\Users\TWINUser13\Downloads\MHV 2024 (1).rvt</t>
   </si>
   <si>
@@ -1350,15 +1299,6 @@
     <t>C:\Users\TWINUser13\Downloads\PUH 2024.rvt</t>
   </si>
   <si>
-    <t>Arab emirates AB2</t>
-  </si>
-  <si>
-    <t>1111-XXXX-XX01-0001-A-P01.32</t>
-  </si>
-  <si>
-    <t>0001-ATXX-XX01-RFI-0001-A-P01.91</t>
-  </si>
-  <si>
     <t>Transmittal/Submittal</t>
   </si>
   <si>
@@ -1380,27 +1320,9 @@
     <t>Transmital</t>
   </si>
   <si>
-    <t>0001-XXXX-XX01-BOM-0001-A-P01.98</t>
-  </si>
-  <si>
-    <t>0001-XXXX-XX01-RFA-0001-A-P01.27</t>
-  </si>
-  <si>
-    <t>0001-XXXX-XX01-ISS-0001-A-P01.57</t>
-  </si>
-  <si>
     <t>Select the parent review</t>
   </si>
   <si>
-    <t>0001-XXXX-XX01-RVW-0001-A-P01.59</t>
-  </si>
-  <si>
-    <t>0001-ATXX-XX01-TRN-0001-A-P01.69</t>
-  </si>
-  <si>
-    <t>0001-ATXX-XX01-SUB-0001-A-P01.89</t>
-  </si>
-  <si>
     <t>While creating new project initiallly Parent Review field will have the default template as Select the Parent review after that you can change with any other id</t>
   </si>
   <si>
@@ -1414,6 +1336,75 @@
   </si>
   <si>
     <t>For Five Step Approval - Name of Approval will be Answered - its default</t>
+  </si>
+  <si>
+    <t>0001-ATXX-XX01-RFI-0001-A-P01.96</t>
+  </si>
+  <si>
+    <t>0001-ATXX-XX01-TRN-0001-A-P01.64</t>
+  </si>
+  <si>
+    <t>Full Automation Demo</t>
+  </si>
+  <si>
+    <t>1111-ABXX-XX01-0001-A-P01.30</t>
+  </si>
+  <si>
+    <t>0001-YTXX-XX01-ISS-0001-A-P01.52</t>
+  </si>
+  <si>
+    <t>0001-IOXX-XX01-RFA-0001-A-P01.24</t>
+  </si>
+  <si>
+    <t>0001-PLXX-XX01-BOM-0001-A-P01.93</t>
+  </si>
+  <si>
+    <t>Alka Rajarajan</t>
+  </si>
+  <si>
+    <t>Balaji Kumar</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Project Tester</t>
+  </si>
+  <si>
+    <t>Watcher2</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>Nesamani Contractor</t>
+  </si>
+  <si>
+    <t>0001-APXX-XX01-SUB-0001-A-P01.83</t>
+  </si>
+  <si>
+    <t>0001-AYTX-XX01-RVW-0001-A-P01.55</t>
+  </si>
+  <si>
+    <t>For Estimated Total, Quoted Total and Actual Total Amount these fields values will be calculated based on before two field this calculation was handled in code level so there is no field added in this sheet</t>
+  </si>
+  <si>
+    <t>RFA code will be Unique</t>
+  </si>
+  <si>
+    <t>Issue code will be Unique</t>
+  </si>
+  <si>
+    <t>Transmittal code will be Unique</t>
+  </si>
+  <si>
+    <t>Submittal code will be Unique</t>
+  </si>
+  <si>
+    <t>RFI code will be Unique</t>
+  </si>
+  <si>
+    <t>Project code will be Unique</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1585,6 +1576,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1902,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7D8262-3FB9-4EA7-BA24-AF35E85ACD1D}">
   <dimension ref="A1:DU13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,10 +2037,10 @@
     </row>
     <row r="2" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:125" x14ac:dyDescent="0.25">
@@ -2056,7 +2048,7 @@
     </row>
     <row r="13" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B13">
         <v>123456</v>
@@ -2074,10 +2066,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1590F75A-691A-4F06-A0D6-97E2B8C650FC}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E1" sqref="E1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,98 +2079,84 @@
     <col min="3" max="3" width="116.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
-        <v>410</v>
-      </c>
-      <c r="E1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C4" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" t="s">
-        <v>430</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C5" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C6" t="s">
         <v>415</v>
       </c>
-      <c r="C4" t="s">
-        <v>429</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>407</v>
+      </c>
+      <c r="C8" t="s">
         <v>417</v>
       </c>
-      <c r="C5" t="s">
-        <v>431</v>
-      </c>
-      <c r="E5" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>419</v>
-      </c>
-      <c r="C6" t="s">
-        <v>432</v>
-      </c>
-      <c r="E6" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>332</v>
-      </c>
-      <c r="C7" t="s">
-        <v>433</v>
-      </c>
-      <c r="E7" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>422</v>
-      </c>
-      <c r="C8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E8" t="s">
-        <v>423</v>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="15" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2191,7 +2169,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2290,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,13 +2363,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="B2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D2" t="s">
         <v>255</v>
@@ -2435,7 +2413,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2448,7 +2426,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>452</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -2461,7 +2439,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,7 +2521,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
@@ -2603,6 +2581,16 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S11" s="5" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="18" spans="15:17" x14ac:dyDescent="0.25">
@@ -2631,10 +2619,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D12559-3BEC-4A49-9DD8-38E929692E89}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2695,7 +2683,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
@@ -2736,6 +2724,16 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>448</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2747,7 +2745,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N23" sqref="N23:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2867,7 +2865,7 @@
         <v>120</v>
       </c>
       <c r="L3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2875,7 +2873,7 @@
         <v>121</v>
       </c>
       <c r="L4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2900,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D35D846-25C7-41D6-9730-C7B818D35A81}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B21"/>
+      <selection activeCell="A24" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2986,7 +2984,7 @@
         <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C2" t="s">
         <v>138</v>
@@ -3061,16 +3059,36 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="13" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>452</v>
+      <c r="B21" s="15" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3196,10 +3214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081DB40F-4E4E-4B24-8430-969987B28590}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,13 +3305,13 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="E2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -3311,7 +3329,7 @@
         <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="L2" t="s">
         <v>27</v>
@@ -3338,6 +3356,11 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
@@ -3357,6 +3380,16 @@
       <c r="C24" s="10"/>
       <c r="D24" s="11" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="15" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -3369,10 +3402,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5927FC2-CAF2-4F62-AF22-9A89FEE1C235}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3419,74 +3452,59 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>438</v>
       </c>
       <c r="C2" t="s">
-        <v>325</v>
+        <v>440</v>
       </c>
       <c r="D2" t="s">
-        <v>342</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>345</v>
+        <v>439</v>
       </c>
       <c r="D3" t="s">
-        <v>341</v>
+        <v>442</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D4" t="s">
-        <v>331</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D5" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3496,10 +3514,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A2A67-EB9E-4636-A126-D12A8CADACD9}">
-  <dimension ref="A1:FS23"/>
+  <dimension ref="A1:FS26"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AY4" sqref="AY4"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3701,19 +3719,19 @@
         <v>166</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="AR1" s="4" t="s">
         <v>287</v>
@@ -3853,22 +3871,22 @@
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G2" t="s">
         <v>151</v>
@@ -3877,20 +3895,41 @@
         <v>53</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
       </c>
       <c r="R2" t="s">
-        <v>326</v>
+        <v>321</v>
+      </c>
+      <c r="S2" t="s">
+        <v>324</v>
+      </c>
+      <c r="T2" t="s">
+        <v>322</v>
       </c>
       <c r="AF2" t="s">
         <v>62</v>
       </c>
+      <c r="AG2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM2">
+        <v>1</v>
+      </c>
       <c r="AR2">
         <v>1</v>
       </c>
@@ -3898,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="AT2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU2">
         <v>1</v>
@@ -4003,19 +4042,19 @@
         <v>1</v>
       </c>
       <c r="CC2">
+        <v>1</v>
+      </c>
+      <c r="CD2">
         <v>0</v>
       </c>
-      <c r="CD2">
-        <v>1</v>
-      </c>
       <c r="CE2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF2">
         <v>1</v>
       </c>
       <c r="CG2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.25">
@@ -4056,10 +4095,10 @@
         <v>156</v>
       </c>
       <c r="R3" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="S3" t="s">
-        <v>157</v>
+        <v>321</v>
       </c>
       <c r="AF3" t="s">
         <v>201</v>
@@ -4196,22 +4235,22 @@
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="F4" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="G4" t="s">
         <v>151</v>
@@ -4223,36 +4262,49 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>174</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>175</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>176</v>
+      </c>
+      <c r="N4" t="s">
+        <v>177</v>
       </c>
       <c r="R4" t="s">
-        <v>157</v>
+        <v>438</v>
       </c>
       <c r="S4" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="T4" t="s">
-        <v>344</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="U4" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC4" s="5"/>
       <c r="AF4" t="s">
-        <v>62</v>
+        <v>203</v>
       </c>
       <c r="AG4" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
       <c r="AH4" t="s">
-        <v>62</v>
+        <v>205</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>206</v>
       </c>
       <c r="AM4">
+        <v>2</v>
+      </c>
+      <c r="AN4">
         <v>1</v>
       </c>
       <c r="AR4">
@@ -4367,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="CC4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD4">
         <v>0</v>
@@ -4376,7 +4428,7 @@
         <v>0</v>
       </c>
       <c r="CF4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG4">
         <v>0</v>
@@ -4384,22 +4436,22 @@
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="G5" t="s">
         <v>151</v>
@@ -4408,53 +4460,19 @@
         <v>53</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
-      </c>
-      <c r="L5" t="s">
-        <v>175</v>
-      </c>
-      <c r="M5" t="s">
-        <v>176</v>
-      </c>
-      <c r="N5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="R5" t="s">
-        <v>327</v>
-      </c>
-      <c r="S5" t="s">
-        <v>157</v>
-      </c>
-      <c r="T5" t="s">
-        <v>329</v>
-      </c>
-      <c r="U5" t="s">
-        <v>326</v>
-      </c>
-      <c r="AC5" s="5"/>
+        <v>321</v>
+      </c>
       <c r="AF5" t="s">
-        <v>203</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>204</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>206</v>
-      </c>
-      <c r="AM5">
-        <v>2</v>
-      </c>
-      <c r="AN5">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="AR5">
         <v>1</v>
@@ -4463,7 +4481,7 @@
         <v>1</v>
       </c>
       <c r="AT5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU5">
         <v>1</v>
@@ -4571,21 +4589,21 @@
         <v>0</v>
       </c>
       <c r="CD5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
@@ -4594,13 +4612,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="E6" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="F6" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="G6" t="s">
         <v>151</v>
@@ -4615,10 +4633,10 @@
         <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="R6" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AF6" t="s">
         <v>62</v>
@@ -4752,7 +4770,7 @@
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
@@ -4761,13 +4779,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="E7" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="F7" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="G7" t="s">
         <v>151</v>
@@ -4782,10 +4800,10 @@
         <v>56</v>
       </c>
       <c r="K7" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="R7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AF7" t="s">
         <v>62</v>
@@ -4931,7 +4949,7 @@
         <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="F8" t="s">
         <v>171</v>
@@ -4952,7 +4970,7 @@
         <v>181</v>
       </c>
       <c r="R8" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AF8" t="s">
         <v>62</v>
@@ -5098,7 +5116,7 @@
         <v>184</v>
       </c>
       <c r="E9" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="F9" t="s">
         <v>178</v>
@@ -5119,7 +5137,7 @@
         <v>186</v>
       </c>
       <c r="R9" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AF9" t="s">
         <v>62</v>
@@ -5286,7 +5304,7 @@
         <v>194</v>
       </c>
       <c r="R10" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AF10" t="s">
         <v>62</v>
@@ -5416,74 +5434,6 @@
       </c>
       <c r="CG10">
         <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="9:175" x14ac:dyDescent="0.25">
-      <c r="I20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AR20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AS20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AT20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AU20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AV20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AW20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="AX20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BM20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BN20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BO20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BP20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BQ20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BR20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="BS20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CA20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CB20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CC20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CD20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CE20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CF20" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="CG20" s="9" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="21" spans="9:175" x14ac:dyDescent="0.25">
@@ -5491,829 +5441,767 @@
         <v>311</v>
       </c>
       <c r="AR21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AS21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AT21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AU21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AV21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AW21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AX21" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="BM21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BN21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BO21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BP21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BQ21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BR21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BS21" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="CA21" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CB21" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CC21" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CD21" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CE21" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CF21" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="CG21" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="CM21" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="CN21" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="CO21" s="19">
-        <v>5</v>
-      </c>
-      <c r="CP21" s="19" t="s">
-        <v>453</v>
-      </c>
-      <c r="CQ21" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="CR21" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="CS21" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="CT21" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="CU21">
-        <v>1</v>
-      </c>
-      <c r="CV21" t="s">
-        <v>58</v>
-      </c>
-      <c r="CW21" t="s">
-        <v>181</v>
-      </c>
-      <c r="CX21" t="s">
-        <v>138</v>
-      </c>
-      <c r="CY21" t="s">
-        <v>51</v>
-      </c>
-      <c r="CZ21" t="s">
-        <v>182</v>
-      </c>
-      <c r="DA21" t="s">
-        <v>183</v>
-      </c>
-      <c r="DD21" t="s">
-        <v>324</v>
-      </c>
-      <c r="DE21" t="s">
-        <v>328</v>
-      </c>
-      <c r="DF21" t="s">
-        <v>344</v>
-      </c>
-      <c r="DG21" t="s">
-        <v>327</v>
-      </c>
-      <c r="DH21" t="s">
-        <v>345</v>
-      </c>
-      <c r="DR21" t="s">
-        <v>207</v>
-      </c>
-      <c r="DS21" t="s">
-        <v>208</v>
-      </c>
-      <c r="DT21" t="s">
-        <v>209</v>
-      </c>
-      <c r="DU21" t="s">
-        <v>210</v>
-      </c>
-      <c r="DV21" t="s">
-        <v>211</v>
-      </c>
-      <c r="DY21">
-        <v>1</v>
-      </c>
-      <c r="DZ21">
-        <v>2</v>
-      </c>
-      <c r="EA21">
-        <v>2</v>
-      </c>
-      <c r="ED21">
-        <v>1</v>
-      </c>
-      <c r="EE21">
-        <v>0</v>
-      </c>
-      <c r="EF21">
-        <v>0</v>
-      </c>
-      <c r="EG21">
-        <v>1</v>
-      </c>
-      <c r="EH21">
-        <v>0</v>
-      </c>
-      <c r="EI21">
-        <v>1</v>
-      </c>
-      <c r="EJ21">
-        <v>0</v>
-      </c>
-      <c r="EK21">
-        <v>1</v>
-      </c>
-      <c r="EL21">
-        <v>1</v>
-      </c>
-      <c r="EM21">
-        <v>1</v>
-      </c>
-      <c r="EN21">
-        <v>1</v>
-      </c>
-      <c r="EO21">
-        <v>1</v>
-      </c>
-      <c r="EP21">
-        <v>1</v>
-      </c>
-      <c r="EQ21">
-        <v>1</v>
-      </c>
-      <c r="ER21">
-        <v>2</v>
-      </c>
-      <c r="ES21">
-        <v>2</v>
-      </c>
-      <c r="ET21">
-        <v>2</v>
-      </c>
-      <c r="EU21">
-        <v>2</v>
-      </c>
-      <c r="EV21">
-        <v>2</v>
-      </c>
-      <c r="EW21">
-        <v>2</v>
-      </c>
-      <c r="EX21">
-        <v>2</v>
-      </c>
-      <c r="EY21" t="s">
-        <v>256</v>
-      </c>
-      <c r="EZ21" t="s">
-        <v>256</v>
-      </c>
-      <c r="FA21" t="s">
-        <v>256</v>
-      </c>
-      <c r="FB21" t="s">
-        <v>256</v>
-      </c>
-      <c r="FC21" t="s">
-        <v>256</v>
-      </c>
-      <c r="FD21" t="s">
-        <v>256</v>
-      </c>
-      <c r="FE21" t="s">
-        <v>256</v>
-      </c>
-      <c r="FF21">
-        <v>2</v>
-      </c>
-      <c r="FG21">
-        <v>2</v>
-      </c>
-      <c r="FH21">
-        <v>2</v>
-      </c>
-      <c r="FI21">
-        <v>2</v>
-      </c>
-      <c r="FJ21">
-        <v>2</v>
-      </c>
-      <c r="FK21">
-        <v>2</v>
-      </c>
-      <c r="FL21">
-        <v>2</v>
-      </c>
-      <c r="FM21">
-        <v>1</v>
-      </c>
-      <c r="FN21">
-        <v>0</v>
-      </c>
-      <c r="FO21">
-        <v>1</v>
-      </c>
-      <c r="FP21">
-        <v>0</v>
-      </c>
-      <c r="FQ21">
-        <v>1</v>
-      </c>
-      <c r="FR21">
-        <v>1</v>
-      </c>
-      <c r="FS21">
-        <v>1</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="9:175" x14ac:dyDescent="0.25">
       <c r="I22" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="AR22" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AS22" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AT22" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AU22" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AV22" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AW22" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AX22" s="11" t="s">
-        <v>316</v>
+        <v>430</v>
       </c>
       <c r="BM22" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BN22" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BO22" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BP22" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BQ22" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BR22" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BS22" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="CA22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CB22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CC22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CD22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CE22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CF22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CG22" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="CM22" s="19" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="CM24" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="CN24" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="CO24" s="19">
+        <v>5</v>
+      </c>
+      <c r="CP24" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="CQ24" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="CR24" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="CS24" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="CT24" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="CU24">
+        <v>1</v>
+      </c>
+      <c r="CV24" t="s">
+        <v>58</v>
+      </c>
+      <c r="CW24" t="s">
+        <v>181</v>
+      </c>
+      <c r="CX24" t="s">
+        <v>138</v>
+      </c>
+      <c r="CY24" t="s">
+        <v>51</v>
+      </c>
+      <c r="CZ24" t="s">
+        <v>182</v>
+      </c>
+      <c r="DA24" t="s">
+        <v>183</v>
+      </c>
+      <c r="DD24" t="s">
+        <v>320</v>
+      </c>
+      <c r="DE24" t="s">
+        <v>323</v>
+      </c>
+      <c r="DF24" t="s">
+        <v>335</v>
+      </c>
+      <c r="DG24" t="s">
+        <v>322</v>
+      </c>
+      <c r="DH24" t="s">
+        <v>336</v>
+      </c>
+      <c r="DR24" t="s">
+        <v>207</v>
+      </c>
+      <c r="DS24" t="s">
+        <v>208</v>
+      </c>
+      <c r="DT24" t="s">
+        <v>209</v>
+      </c>
+      <c r="DU24" t="s">
+        <v>210</v>
+      </c>
+      <c r="DV24" t="s">
+        <v>211</v>
+      </c>
+      <c r="DY24">
+        <v>1</v>
+      </c>
+      <c r="DZ24">
+        <v>2</v>
+      </c>
+      <c r="EA24">
+        <v>2</v>
+      </c>
+      <c r="ED24">
+        <v>1</v>
+      </c>
+      <c r="EE24">
+        <v>0</v>
+      </c>
+      <c r="EF24">
+        <v>0</v>
+      </c>
+      <c r="EG24">
+        <v>1</v>
+      </c>
+      <c r="EH24">
+        <v>0</v>
+      </c>
+      <c r="EI24">
+        <v>1</v>
+      </c>
+      <c r="EJ24">
+        <v>0</v>
+      </c>
+      <c r="EK24">
+        <v>1</v>
+      </c>
+      <c r="EL24">
+        <v>1</v>
+      </c>
+      <c r="EM24">
+        <v>1</v>
+      </c>
+      <c r="EN24">
+        <v>1</v>
+      </c>
+      <c r="EO24">
+        <v>1</v>
+      </c>
+      <c r="EP24">
+        <v>1</v>
+      </c>
+      <c r="EQ24">
+        <v>1</v>
+      </c>
+      <c r="ER24">
+        <v>2</v>
+      </c>
+      <c r="ES24">
+        <v>2</v>
+      </c>
+      <c r="ET24">
+        <v>2</v>
+      </c>
+      <c r="EU24">
+        <v>2</v>
+      </c>
+      <c r="EV24">
+        <v>2</v>
+      </c>
+      <c r="EW24">
+        <v>2</v>
+      </c>
+      <c r="EX24">
+        <v>2</v>
+      </c>
+      <c r="EY24" t="s">
+        <v>256</v>
+      </c>
+      <c r="EZ24" t="s">
+        <v>256</v>
+      </c>
+      <c r="FA24" t="s">
+        <v>256</v>
+      </c>
+      <c r="FB24" t="s">
+        <v>256</v>
+      </c>
+      <c r="FC24" t="s">
+        <v>256</v>
+      </c>
+      <c r="FD24" t="s">
+        <v>256</v>
+      </c>
+      <c r="FE24" t="s">
+        <v>256</v>
+      </c>
+      <c r="FF24">
+        <v>2</v>
+      </c>
+      <c r="FG24">
+        <v>2</v>
+      </c>
+      <c r="FH24">
+        <v>2</v>
+      </c>
+      <c r="FI24">
+        <v>2</v>
+      </c>
+      <c r="FJ24">
+        <v>2</v>
+      </c>
+      <c r="FK24">
+        <v>2</v>
+      </c>
+      <c r="FL24">
+        <v>2</v>
+      </c>
+      <c r="FM24">
+        <v>1</v>
+      </c>
+      <c r="FN24">
+        <v>0</v>
+      </c>
+      <c r="FO24">
+        <v>1</v>
+      </c>
+      <c r="FP24">
+        <v>0</v>
+      </c>
+      <c r="FQ24">
+        <v>1</v>
+      </c>
+      <c r="FR24">
+        <v>1</v>
+      </c>
+      <c r="FS24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="CM25" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="CN22" s="19" t="s">
+      <c r="CN25" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="CO22" s="19">
+      <c r="CO25" s="19">
         <v>6</v>
       </c>
-      <c r="CP22" s="19" t="s">
-        <v>454</v>
-      </c>
-      <c r="CQ22" s="19" t="s">
+      <c r="CP25" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="CQ25" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="CR22" s="19" t="s">
+      <c r="CR25" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="CS22" s="19" t="s">
+      <c r="CS25" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="CT22" s="19" t="s">
+      <c r="CT25" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="CU22">
-        <v>1</v>
-      </c>
-      <c r="CV22" t="s">
+      <c r="CU25">
+        <v>1</v>
+      </c>
+      <c r="CV25" t="s">
         <v>59</v>
       </c>
-      <c r="CW22" t="s">
+      <c r="CW25" t="s">
         <v>186</v>
       </c>
-      <c r="CX22" t="s">
+      <c r="CX25" t="s">
         <v>187</v>
       </c>
-      <c r="CY22" t="s">
+      <c r="CY25" t="s">
         <v>188</v>
       </c>
-      <c r="CZ22" t="s">
+      <c r="CZ25" t="s">
         <v>189</v>
       </c>
-      <c r="DA22" t="s">
+      <c r="DA25" t="s">
         <v>190</v>
       </c>
-      <c r="DB22" t="s">
+      <c r="DB25" t="s">
         <v>191</v>
       </c>
-      <c r="DD22" t="s">
-        <v>326</v>
-      </c>
-      <c r="DE22" t="s">
+      <c r="DD25" t="s">
+        <v>321</v>
+      </c>
+      <c r="DE25" t="s">
         <v>157</v>
       </c>
-      <c r="DF22" t="s">
+      <c r="DF25" t="s">
+        <v>320</v>
+      </c>
+      <c r="DG25" t="s">
+        <v>323</v>
+      </c>
+      <c r="DH25" t="s">
+        <v>336</v>
+      </c>
+      <c r="DI25" t="s">
         <v>324</v>
       </c>
-      <c r="DG22" t="s">
-        <v>328</v>
-      </c>
-      <c r="DH22" t="s">
+      <c r="DO25" s="5"/>
+      <c r="DR25" t="s">
+        <v>62</v>
+      </c>
+      <c r="DS25" t="s">
+        <v>234</v>
+      </c>
+      <c r="DT25" t="s">
+        <v>235</v>
+      </c>
+      <c r="DU25" t="s">
+        <v>236</v>
+      </c>
+      <c r="DV25" t="s">
+        <v>62</v>
+      </c>
+      <c r="DW25" t="s">
+        <v>237</v>
+      </c>
+      <c r="DY25">
+        <v>1</v>
+      </c>
+      <c r="DZ25">
+        <v>1</v>
+      </c>
+      <c r="EA25">
+        <v>2</v>
+      </c>
+      <c r="EB25">
+        <v>2</v>
+      </c>
+      <c r="ED25">
+        <v>1</v>
+      </c>
+      <c r="EE25">
+        <v>1</v>
+      </c>
+      <c r="EF25">
+        <v>1</v>
+      </c>
+      <c r="EG25">
+        <v>1</v>
+      </c>
+      <c r="EH25">
+        <v>0</v>
+      </c>
+      <c r="EI25">
+        <v>0</v>
+      </c>
+      <c r="EJ25">
+        <v>1</v>
+      </c>
+      <c r="EK25">
+        <v>1</v>
+      </c>
+      <c r="EL25">
+        <v>1</v>
+      </c>
+      <c r="EM25">
+        <v>1</v>
+      </c>
+      <c r="EN25">
+        <v>1</v>
+      </c>
+      <c r="EO25">
+        <v>1</v>
+      </c>
+      <c r="EP25">
+        <v>1</v>
+      </c>
+      <c r="EQ25">
+        <v>1</v>
+      </c>
+      <c r="ER25">
+        <v>2</v>
+      </c>
+      <c r="ES25">
+        <v>2</v>
+      </c>
+      <c r="ET25">
+        <v>2</v>
+      </c>
+      <c r="EU25">
+        <v>2</v>
+      </c>
+      <c r="EV25">
+        <v>2</v>
+      </c>
+      <c r="EW25">
+        <v>2</v>
+      </c>
+      <c r="EX25">
+        <v>2</v>
+      </c>
+      <c r="EY25" t="s">
+        <v>256</v>
+      </c>
+      <c r="EZ25" t="s">
+        <v>256</v>
+      </c>
+      <c r="FA25" t="s">
+        <v>256</v>
+      </c>
+      <c r="FB25" t="s">
+        <v>256</v>
+      </c>
+      <c r="FC25" t="s">
+        <v>256</v>
+      </c>
+      <c r="FD25" t="s">
+        <v>256</v>
+      </c>
+      <c r="FE25" t="s">
+        <v>256</v>
+      </c>
+      <c r="FF25">
+        <v>2</v>
+      </c>
+      <c r="FG25">
+        <v>2</v>
+      </c>
+      <c r="FH25">
+        <v>2</v>
+      </c>
+      <c r="FI25">
+        <v>2</v>
+      </c>
+      <c r="FJ25">
+        <v>2</v>
+      </c>
+      <c r="FK25">
+        <v>2</v>
+      </c>
+      <c r="FL25">
+        <v>2</v>
+      </c>
+      <c r="FM25">
+        <v>1</v>
+      </c>
+      <c r="FN25">
+        <v>0</v>
+      </c>
+      <c r="FO25">
+        <v>0</v>
+      </c>
+      <c r="FP25">
+        <v>1</v>
+      </c>
+      <c r="FQ25">
+        <v>0</v>
+      </c>
+      <c r="FR25">
+        <v>0</v>
+      </c>
+      <c r="FS25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="9:175" x14ac:dyDescent="0.25">
+      <c r="CM26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="CN26" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="CO26" s="19">
+        <v>7</v>
+      </c>
+      <c r="CP26" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="CQ26" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="CR26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="CS26" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="CT26" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="CU26">
+        <v>0</v>
+      </c>
+      <c r="CV26" t="s">
+        <v>60</v>
+      </c>
+      <c r="CW26" t="s">
+        <v>194</v>
+      </c>
+      <c r="CX26" t="s">
+        <v>195</v>
+      </c>
+      <c r="CY26" t="s">
+        <v>196</v>
+      </c>
+      <c r="CZ26" t="s">
+        <v>197</v>
+      </c>
+      <c r="DA26" t="s">
+        <v>198</v>
+      </c>
+      <c r="DB26" t="s">
+        <v>199</v>
+      </c>
+      <c r="DC26" t="s">
+        <v>200</v>
+      </c>
+      <c r="DD26" t="s">
+        <v>335</v>
+      </c>
+      <c r="DE26" t="s">
+        <v>157</v>
+      </c>
+      <c r="DF26" t="s">
+        <v>336</v>
+      </c>
+      <c r="DG26" t="s">
+        <v>321</v>
+      </c>
+      <c r="DH26" t="s">
+        <v>337</v>
+      </c>
+      <c r="DI26" t="s">
+        <v>323</v>
+      </c>
+      <c r="DJ26" t="s">
+        <v>320</v>
+      </c>
+      <c r="DO26" s="5"/>
+      <c r="DP26" s="5"/>
+      <c r="DR26" t="s">
+        <v>339</v>
+      </c>
+      <c r="DS26" t="s">
+        <v>340</v>
+      </c>
+      <c r="DT26" t="s">
+        <v>341</v>
+      </c>
+      <c r="DU26" t="s">
+        <v>342</v>
+      </c>
+      <c r="DV26" t="s">
+        <v>343</v>
+      </c>
+      <c r="DW26" t="s">
+        <v>344</v>
+      </c>
+      <c r="DX26" t="s">
         <v>345</v>
       </c>
-      <c r="DI22" t="s">
-        <v>329</v>
-      </c>
-      <c r="DO22" s="5"/>
-      <c r="DR22" t="s">
-        <v>62</v>
-      </c>
-      <c r="DS22" t="s">
-        <v>234</v>
-      </c>
-      <c r="DT22" t="s">
-        <v>235</v>
-      </c>
-      <c r="DU22" t="s">
-        <v>236</v>
-      </c>
-      <c r="DV22" t="s">
-        <v>62</v>
-      </c>
-      <c r="DW22" t="s">
-        <v>237</v>
-      </c>
-      <c r="DY22">
-        <v>1</v>
-      </c>
-      <c r="DZ22">
-        <v>1</v>
-      </c>
-      <c r="EA22">
-        <v>2</v>
-      </c>
-      <c r="EB22">
-        <v>2</v>
-      </c>
-      <c r="ED22">
-        <v>1</v>
-      </c>
-      <c r="EE22">
-        <v>1</v>
-      </c>
-      <c r="EF22">
-        <v>1</v>
-      </c>
-      <c r="EG22">
-        <v>1</v>
-      </c>
-      <c r="EH22">
+      <c r="DY26">
+        <v>2</v>
+      </c>
+      <c r="DZ26">
+        <v>1</v>
+      </c>
+      <c r="EA26">
+        <v>1</v>
+      </c>
+      <c r="EB26">
+        <v>2</v>
+      </c>
+      <c r="EC26">
+        <v>2</v>
+      </c>
+      <c r="ED26">
+        <v>2</v>
+      </c>
+      <c r="EE26">
+        <v>1</v>
+      </c>
+      <c r="EF26">
+        <v>1</v>
+      </c>
+      <c r="EG26">
         <v>0</v>
       </c>
-      <c r="EI22">
+      <c r="EH26">
         <v>0</v>
       </c>
-      <c r="EJ22">
-        <v>1</v>
-      </c>
-      <c r="EK22">
-        <v>1</v>
-      </c>
-      <c r="EL22">
-        <v>1</v>
-      </c>
-      <c r="EM22">
-        <v>1</v>
-      </c>
-      <c r="EN22">
-        <v>1</v>
-      </c>
-      <c r="EO22">
-        <v>1</v>
-      </c>
-      <c r="EP22">
-        <v>1</v>
-      </c>
-      <c r="EQ22">
-        <v>1</v>
-      </c>
-      <c r="ER22">
-        <v>2</v>
-      </c>
-      <c r="ES22">
-        <v>2</v>
-      </c>
-      <c r="ET22">
-        <v>2</v>
-      </c>
-      <c r="EU22">
-        <v>2</v>
-      </c>
-      <c r="EV22">
-        <v>2</v>
-      </c>
-      <c r="EW22">
-        <v>2</v>
-      </c>
-      <c r="EX22">
-        <v>2</v>
-      </c>
-      <c r="EY22" t="s">
-        <v>256</v>
-      </c>
-      <c r="EZ22" t="s">
-        <v>256</v>
-      </c>
-      <c r="FA22" t="s">
-        <v>256</v>
-      </c>
-      <c r="FB22" t="s">
-        <v>256</v>
-      </c>
-      <c r="FC22" t="s">
-        <v>256</v>
-      </c>
-      <c r="FD22" t="s">
-        <v>256</v>
-      </c>
-      <c r="FE22" t="s">
-        <v>256</v>
-      </c>
-      <c r="FF22">
-        <v>2</v>
-      </c>
-      <c r="FG22">
-        <v>2</v>
-      </c>
-      <c r="FH22">
-        <v>2</v>
-      </c>
-      <c r="FI22">
-        <v>2</v>
-      </c>
-      <c r="FJ22">
-        <v>2</v>
-      </c>
-      <c r="FK22">
-        <v>2</v>
-      </c>
-      <c r="FL22">
-        <v>2</v>
-      </c>
-      <c r="FM22">
-        <v>1</v>
-      </c>
-      <c r="FN22">
+      <c r="EI26">
+        <v>1</v>
+      </c>
+      <c r="EJ26">
+        <v>1</v>
+      </c>
+      <c r="EK26">
+        <v>1</v>
+      </c>
+      <c r="EL26">
+        <v>1</v>
+      </c>
+      <c r="EM26">
+        <v>1</v>
+      </c>
+      <c r="EN26">
+        <v>1</v>
+      </c>
+      <c r="EO26">
+        <v>1</v>
+      </c>
+      <c r="EP26">
+        <v>1</v>
+      </c>
+      <c r="EQ26">
+        <v>1</v>
+      </c>
+      <c r="ER26">
+        <v>2</v>
+      </c>
+      <c r="ES26">
+        <v>2</v>
+      </c>
+      <c r="ET26">
+        <v>2</v>
+      </c>
+      <c r="EU26">
+        <v>2</v>
+      </c>
+      <c r="EV26">
+        <v>2</v>
+      </c>
+      <c r="EW26">
+        <v>2</v>
+      </c>
+      <c r="EX26">
+        <v>2</v>
+      </c>
+      <c r="EY26" t="s">
+        <v>256</v>
+      </c>
+      <c r="EZ26" t="s">
+        <v>256</v>
+      </c>
+      <c r="FA26" t="s">
+        <v>256</v>
+      </c>
+      <c r="FB26" t="s">
+        <v>256</v>
+      </c>
+      <c r="FC26" t="s">
+        <v>256</v>
+      </c>
+      <c r="FD26" t="s">
+        <v>256</v>
+      </c>
+      <c r="FE26" t="s">
+        <v>256</v>
+      </c>
+      <c r="FF26">
+        <v>2</v>
+      </c>
+      <c r="FG26">
+        <v>2</v>
+      </c>
+      <c r="FH26">
+        <v>2</v>
+      </c>
+      <c r="FI26">
+        <v>2</v>
+      </c>
+      <c r="FJ26">
+        <v>2</v>
+      </c>
+      <c r="FK26">
+        <v>2</v>
+      </c>
+      <c r="FL26">
+        <v>2</v>
+      </c>
+      <c r="FM26">
         <v>0</v>
       </c>
-      <c r="FO22">
+      <c r="FN26">
+        <v>1</v>
+      </c>
+      <c r="FO26">
         <v>0</v>
       </c>
-      <c r="FP22">
-        <v>1</v>
-      </c>
-      <c r="FQ22">
+      <c r="FP26">
+        <v>1</v>
+      </c>
+      <c r="FQ26">
         <v>0</v>
       </c>
-      <c r="FR22">
-        <v>0</v>
-      </c>
-      <c r="FS22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="9:175" x14ac:dyDescent="0.25">
-      <c r="I23" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="BM23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="BN23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="BO23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="BP23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="BQ23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="BR23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="BS23" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="CM23" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="CN23" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="CO23" s="19">
-        <v>7</v>
-      </c>
-      <c r="CP23" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="CQ23" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="CR23" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="CS23" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="CT23" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="CU23">
-        <v>0</v>
-      </c>
-      <c r="CV23" t="s">
-        <v>60</v>
-      </c>
-      <c r="CW23" t="s">
-        <v>194</v>
-      </c>
-      <c r="CX23" t="s">
-        <v>195</v>
-      </c>
-      <c r="CY23" t="s">
-        <v>196</v>
-      </c>
-      <c r="CZ23" t="s">
-        <v>197</v>
-      </c>
-      <c r="DA23" t="s">
-        <v>198</v>
-      </c>
-      <c r="DB23" t="s">
-        <v>199</v>
-      </c>
-      <c r="DC23" t="s">
-        <v>200</v>
-      </c>
-      <c r="DD23" t="s">
-        <v>344</v>
-      </c>
-      <c r="DE23" t="s">
-        <v>157</v>
-      </c>
-      <c r="DF23" t="s">
-        <v>345</v>
-      </c>
-      <c r="DG23" t="s">
-        <v>326</v>
-      </c>
-      <c r="DH23" t="s">
-        <v>346</v>
-      </c>
-      <c r="DI23" t="s">
-        <v>328</v>
-      </c>
-      <c r="DJ23" t="s">
-        <v>324</v>
-      </c>
-      <c r="DO23" s="5"/>
-      <c r="DP23" s="5"/>
-      <c r="DR23" t="s">
-        <v>348</v>
-      </c>
-      <c r="DS23" t="s">
-        <v>349</v>
-      </c>
-      <c r="DT23" t="s">
-        <v>350</v>
-      </c>
-      <c r="DU23" t="s">
-        <v>351</v>
-      </c>
-      <c r="DV23" t="s">
-        <v>352</v>
-      </c>
-      <c r="DW23" t="s">
-        <v>353</v>
-      </c>
-      <c r="DX23" t="s">
-        <v>354</v>
-      </c>
-      <c r="DY23">
-        <v>2</v>
-      </c>
-      <c r="DZ23">
-        <v>1</v>
-      </c>
-      <c r="EA23">
-        <v>1</v>
-      </c>
-      <c r="EB23">
-        <v>2</v>
-      </c>
-      <c r="EC23">
-        <v>2</v>
-      </c>
-      <c r="ED23">
-        <v>2</v>
-      </c>
-      <c r="EE23">
-        <v>1</v>
-      </c>
-      <c r="EF23">
-        <v>1</v>
-      </c>
-      <c r="EG23">
-        <v>0</v>
-      </c>
-      <c r="EH23">
-        <v>0</v>
-      </c>
-      <c r="EI23">
-        <v>1</v>
-      </c>
-      <c r="EJ23">
-        <v>1</v>
-      </c>
-      <c r="EK23">
-        <v>1</v>
-      </c>
-      <c r="EL23">
-        <v>1</v>
-      </c>
-      <c r="EM23">
-        <v>1</v>
-      </c>
-      <c r="EN23">
-        <v>1</v>
-      </c>
-      <c r="EO23">
-        <v>1</v>
-      </c>
-      <c r="EP23">
-        <v>1</v>
-      </c>
-      <c r="EQ23">
-        <v>1</v>
-      </c>
-      <c r="ER23">
-        <v>2</v>
-      </c>
-      <c r="ES23">
-        <v>2</v>
-      </c>
-      <c r="ET23">
-        <v>2</v>
-      </c>
-      <c r="EU23">
-        <v>2</v>
-      </c>
-      <c r="EV23">
-        <v>2</v>
-      </c>
-      <c r="EW23">
-        <v>2</v>
-      </c>
-      <c r="EX23">
-        <v>2</v>
-      </c>
-      <c r="EY23" t="s">
-        <v>256</v>
-      </c>
-      <c r="EZ23" t="s">
-        <v>256</v>
-      </c>
-      <c r="FA23" t="s">
-        <v>256</v>
-      </c>
-      <c r="FB23" t="s">
-        <v>256</v>
-      </c>
-      <c r="FC23" t="s">
-        <v>256</v>
-      </c>
-      <c r="FD23" t="s">
-        <v>256</v>
-      </c>
-      <c r="FE23" t="s">
-        <v>256</v>
-      </c>
-      <c r="FF23">
-        <v>2</v>
-      </c>
-      <c r="FG23">
-        <v>2</v>
-      </c>
-      <c r="FH23">
-        <v>2</v>
-      </c>
-      <c r="FI23">
-        <v>2</v>
-      </c>
-      <c r="FJ23">
-        <v>2</v>
-      </c>
-      <c r="FK23">
-        <v>2</v>
-      </c>
-      <c r="FL23">
-        <v>2</v>
-      </c>
-      <c r="FM23">
-        <v>0</v>
-      </c>
-      <c r="FN23">
-        <v>1</v>
-      </c>
-      <c r="FO23">
-        <v>0</v>
-      </c>
-      <c r="FP23">
-        <v>1</v>
-      </c>
-      <c r="FQ23">
-        <v>0</v>
-      </c>
-      <c r="FR23">
-        <v>1</v>
-      </c>
-      <c r="FS23">
+      <c r="FR26">
+        <v>1</v>
+      </c>
+      <c r="FS26">
         <v>0</v>
       </c>
     </row>
@@ -6325,10 +6213,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6434F126-62F9-459C-95C6-E13119077C7A}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C25" sqref="C25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6351,22 +6239,22 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>82</v>
@@ -6384,7 +6272,7 @@
         <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>241</v>
@@ -6396,7 +6284,7 @@
         <v>74</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>78</v>
@@ -6407,22 +6295,22 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D2" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G2">
         <v>31</v>
@@ -6434,16 +6322,16 @@
         <v>2024</v>
       </c>
       <c r="J2" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="K2" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="L2" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="M2" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="N2" t="s">
         <v>179</v>
@@ -6455,10 +6343,20 @@
         <v>97</v>
       </c>
       <c r="Q2" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="R2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="15" t="s">
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -6468,10 +6366,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414E0F92-D9D0-4190-8614-CA716F440B10}">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6501,22 +6399,22 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>46</v>
@@ -6540,34 +6438,34 @@
         <v>74</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>78</v>
@@ -6584,25 +6482,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="D2" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="E2" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="H2" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="I2" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="J2">
         <v>30</v>
@@ -6647,7 +6545,7 @@
         <v>10</v>
       </c>
       <c r="X2" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="Y2" t="s">
         <v>21</v>
@@ -6655,7 +6553,17 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="X14" t="s">
-        <v>368</v>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="15" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -6665,10 +6573,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D41744-C308-4057-8F9F-E4AB4E75C5B1}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6685,16 +6593,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>46</v>
@@ -6711,28 +6619,38 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="D2" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E2" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="F2" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="G2" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="15" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -6744,8 +6662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF25439C-7A3F-4F80-9A72-7D557AD94E32}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6763,10 +6681,10 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>67</v>
@@ -6797,54 +6715,54 @@
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>126</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="V1" s="4"/>
       <c r="W1" s="4" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6865,16 +6783,16 @@
         <v>2024</v>
       </c>
       <c r="I2" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="J2" t="s">
         <v>184</v>
       </c>
       <c r="K2" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="M2" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="N2">
         <v>10</v>
@@ -6883,22 +6801,22 @@
         <v>100</v>
       </c>
       <c r="P2" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="R2" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="S2">
         <v>10</v>
       </c>
       <c r="T2" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="U2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="W2" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="X2">
         <v>2</v>
@@ -6907,10 +6825,10 @@
         <v>24</v>
       </c>
       <c r="Z2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="AB2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel updation fro Creating new Project
</commit_message>
<xml_diff>
--- a/Excel/TigerKrionDataSheet.xlsx
+++ b/Excel/TigerKrionDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TWINUser13\eclipse-workspace\check\Krion_6D_Consultation-main\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6445EFE2-7FA0-49EF-87CD-2BEFB9D7A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17120F5C-4CA3-45F2-842A-D94231F710E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{1164447D-6810-431B-8BC4-5F1CA151FBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -1894,7 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7D8262-3FB9-4EA7-BA24-AF35E85ACD1D}">
   <dimension ref="A1:DU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -3216,8 +3216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081DB40F-4E4E-4B24-8430-969987B28590}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,7 +3308,7 @@
         <v>434</v>
       </c>
       <c r="D2" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="E2" t="s">
         <v>319</v>
@@ -3358,9 +3358,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>433</v>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>